<commit_message>
Okno 02.12.2025 - aktualizacja EXCEL PL
</commit_message>
<xml_diff>
--- a/assets/excel/pl/wskazniki_globalne.xlsx
+++ b/assets/excel/pl/wskazniki_globalne.xlsx
@@ -1219,43 +1219,43 @@
     <t>PM 10 - wg aglomeracji</t>
   </si>
   <si>
-    <t>Aglomeracja Białostocka</t>
+    <t>aglomeracja białostocka</t>
   </si>
   <si>
     <t>µg/m3</t>
   </si>
   <si>
-    <t>Aglomeracja Bydgoska</t>
-  </si>
-  <si>
-    <t>Aglomeracja Górnośląska</t>
-  </si>
-  <si>
-    <t>Aglomeracja Krakowska</t>
-  </si>
-  <si>
-    <t>Aglomeracja Lubelska</t>
-  </si>
-  <si>
-    <t>Aglomeracja Łódzka</t>
-  </si>
-  <si>
-    <t>Aglomeracja Poznańska</t>
-  </si>
-  <si>
-    <t>Aglomeracja Rybnicko-Jastrzębska</t>
-  </si>
-  <si>
-    <t>Aglomeracja Szczecińska</t>
-  </si>
-  <si>
-    <t>Aglomeracja Trójmiejska</t>
-  </si>
-  <si>
-    <t>Aglomeracja Warszawska</t>
-  </si>
-  <si>
-    <t>Aglomeracja Wrocławska</t>
+    <t>aglomeracja bydgoska</t>
+  </si>
+  <si>
+    <t>aglomeracja górnośląska</t>
+  </si>
+  <si>
+    <t>aglomeracja krakowska</t>
+  </si>
+  <si>
+    <t>aglomeracja lubelska</t>
+  </si>
+  <si>
+    <t>aglomeracja łódzka</t>
+  </si>
+  <si>
+    <t>aglomeracja poznańska</t>
+  </si>
+  <si>
+    <t>aglomeracja rybnicko-jastrzębska</t>
+  </si>
+  <si>
+    <t>aglomeracja szczecińska</t>
+  </si>
+  <si>
+    <t>aglomeracja trójmiejska</t>
+  </si>
+  <si>
+    <t>aglomeracja warszawska</t>
+  </si>
+  <si>
+    <t>aglomeracja wrocławska</t>
   </si>
   <si>
     <t xml:space="preserve"> PM 2.5 - wg aglomeracji</t>
@@ -1684,7 +1684,7 @@
     <t>100% rejestracja zgonów</t>
   </si>
   <si>
-    <t>Ostatnia aktualizacja: 03-12-2025, 09:19</t>
+    <t>Ostatnia aktualizacja: 08-12-2025, 11:48</t>
   </si>
 </sst>
 </file>
@@ -2235,7 +2235,7 @@
   <dimension ref="A1:U479"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -21065,7 +21065,7 @@
         <v>399</v>
       </c>
       <c r="F343" s="4">
-        <v>65.900000000000006</v>
+        <v>65.8</v>
       </c>
       <c r="G343" s="4">
         <v>64.7</v>
@@ -21130,7 +21130,7 @@
         <v>399</v>
       </c>
       <c r="F344" s="4">
-        <v>32</v>
+        <v>57.7</v>
       </c>
       <c r="G344" s="4">
         <v>32.5</v>
@@ -21195,7 +21195,7 @@
         <v>399</v>
       </c>
       <c r="F345" s="4">
-        <v>42.7</v>
+        <v>31.2</v>
       </c>
       <c r="G345" s="4">
         <v>40.5</v>
@@ -21260,7 +21260,7 @@
         <v>399</v>
       </c>
       <c r="F346" s="4">
-        <v>38</v>
+        <v>25.4</v>
       </c>
       <c r="G346" s="4">
         <v>39</v>
@@ -21325,7 +21325,7 @@
         <v>399</v>
       </c>
       <c r="F347" s="4">
-        <v>57.7</v>
+        <v>38</v>
       </c>
       <c r="G347" s="4">
         <v>51</v>
@@ -21390,7 +21390,7 @@
         <v>399</v>
       </c>
       <c r="F348" s="4">
-        <v>31.2</v>
+        <v>54.9</v>
       </c>
       <c r="G348" s="4">
         <v>28.3</v>
@@ -21455,7 +21455,7 @@
         <v>399</v>
       </c>
       <c r="F349" s="4">
-        <v>25.4</v>
+        <v>23.7</v>
       </c>
       <c r="G349" s="4">
         <v>23.4</v>
@@ -21520,7 +21520,7 @@
         <v>399</v>
       </c>
       <c r="F350" s="4">
-        <v>38</v>
+        <v>27.7</v>
       </c>
       <c r="G350" s="4">
         <v>37.6</v>
@@ -21585,7 +21585,7 @@
         <v>399</v>
       </c>
       <c r="F351" s="4">
-        <v>54.9</v>
+        <v>42.5</v>
       </c>
       <c r="G351" s="4">
         <v>45.5</v>
@@ -21650,7 +21650,7 @@
         <v>399</v>
       </c>
       <c r="F352" s="4">
-        <v>23.7</v>
+        <v>50.9</v>
       </c>
       <c r="G352" s="4">
         <v>27.1</v>
@@ -21715,7 +21715,7 @@
         <v>399</v>
       </c>
       <c r="F353" s="4">
-        <v>27.7</v>
+        <v>25.1</v>
       </c>
       <c r="G353" s="4">
         <v>17.399999999999999</v>
@@ -21780,7 +21780,7 @@
         <v>399</v>
       </c>
       <c r="F354" s="4">
-        <v>42.5</v>
+        <v>26.2</v>
       </c>
       <c r="G354" s="4">
         <v>36.700000000000003</v>
@@ -21844,9 +21844,7 @@
       <c r="E355" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="F355" s="4">
-        <v>50.9</v>
-      </c>
+      <c r="F355" s="3"/>
       <c r="G355" s="4">
         <v>45.1</v>
       </c>
@@ -21910,7 +21908,7 @@
         <v>399</v>
       </c>
       <c r="F356" s="4">
-        <v>25.1</v>
+        <v>44.3</v>
       </c>
       <c r="G356" s="4">
         <v>23.2</v>
@@ -21975,7 +21973,7 @@
         <v>399</v>
       </c>
       <c r="F357" s="4">
-        <v>26.2</v>
+        <v>19.3</v>
       </c>
       <c r="G357" s="4">
         <v>27.5</v>
@@ -22039,7 +22037,9 @@
       <c r="E358" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="F358" s="3"/>
+      <c r="F358" s="4">
+        <v>20.3</v>
+      </c>
       <c r="G358" s="4">
         <v>27.5</v>
       </c>
@@ -22103,7 +22103,7 @@
         <v>399</v>
       </c>
       <c r="F359" s="4">
-        <v>44.3</v>
+        <v>30.9</v>
       </c>
       <c r="G359" s="4">
         <v>33</v>
@@ -22168,7 +22168,7 @@
         <v>399</v>
       </c>
       <c r="F360" s="4">
-        <v>19.3</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="G360" s="4">
         <v>18.8</v>
@@ -22232,9 +22232,7 @@
       <c r="E361" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="F361" s="4">
-        <v>20.3</v>
-      </c>
+      <c r="F361" s="3"/>
       <c r="G361" s="4">
         <v>18.2</v>
       </c>
@@ -22297,9 +22295,7 @@
       <c r="E362" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="F362" s="4">
-        <v>30.9</v>
-      </c>
+      <c r="F362" s="3"/>
       <c r="G362" s="4">
         <v>28</v>
       </c>
@@ -22362,9 +22358,7 @@
       <c r="E363" s="3" t="s">
         <v>399</v>
       </c>
-      <c r="F363" s="4">
-        <v>34.799999999999997</v>
-      </c>
+      <c r="F363" s="3"/>
       <c r="G363" s="4">
         <v>30.3</v>
       </c>

</xml_diff>